<commit_message>
commit "Batu Kawan 2018-2020"
</commit_message>
<xml_diff>
--- a/2020_Gallery.xlsx
+++ b/2020_Gallery.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KN\Desktop\SPORTS CLUB 2019-2020\06 Programming\02_Workshop_Material\01_Sphinx\Vir_Pro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE1CA935-99BF-45CE-9D1C-4110E000D1FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7631F75-4C19-468D-B927-BF5F531DDA74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1692" uniqueCount="1604">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2079" uniqueCount="1720">
   <si>
     <t>x</t>
   </si>
@@ -21050,6 +21050,1615 @@
 6.2 million
 K. Project Details
 450mm bored pile, RC Wall, Earthwork"</t>
+  </si>
+  <si>
+    <t>18E1419</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+DAM Safety Review of Semenyih DAM 2018
+B. Client
+Pengurusan Air Selangor Sdn Bhd
+C. Type of Development
+-
+D. Geology Formation
+Gramite
+E. Land Area (acre)
+-
+F. How Many Blocks &amp; Storeys
+-
+G. Total Build-up Area (sq.m)
+-
+H. Foundation System used
+-
+I. Basement Levels &amp; Depth
+-
+J. Estimated Total Project Cost
+-
+K. Project Details
+Safety Review of Semenyih Dam"</t>
+  </si>
+  <si>
+    <t>18G1441</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Geotechnical Input for 845 Acres Mixed Industry &amp; Commercial Development at Bidor
+B. Client
+Premium Medical Product Sdn Bhd
+C. Type of Development
+-
+D. Geology Formation
+-
+E. Land Area (acre)
+845
+F. How Many Blocks &amp; Storeys
+4 Storeys Hostel (13 Blks), 5 Storeys Industrial Block (5 Blks) &amp; 7 Storeys Industrial Block (8 Blks)
+G. Total Build-up Area (sq.m)
+498
+H. Foundation System used
+-
+I. Basement Levels &amp; Depth
+-
+J. Estimated Total Project Cost
+-
+K. Project Details
+-"</t>
+  </si>
+  <si>
+    <t>18G1439</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+L3A Bukit Jelutong, Shah Alam
+B. Client
+G&amp;P Infra Sdn Bhd
+C. Type of Development
+Residential
+D. Geology Formation
+Kenny Hill
+E. Land Area (acre)
+8.421
+F. How Many Blocks &amp; Storeys
+46 Units
+G. Total Build-up Area (sq.m)
+16000 to 17000
+H. Foundation System used
+-
+I. Basement Levels &amp; Depth
+-
+J. Estimated Total Project Cost
+-
+K. Project Details
+Pile Design"</t>
+  </si>
+  <si>
+    <t>"18E1419
+A. Project Tittle
+DAM Safety Review of Semenyih DAM 2018
+B. Client
+Pengurusan Air Selangor Sdn Bhd
+C. Type of Development
+-
+D. Geology Formation
+E. Land Area (acre)
+F. How Many Blocks &amp; Storeys
+G. Total Build-up Area (sq.m)
+H. Foundation System used
+I. Basement Levels &amp; Depth
+J. Estimated Total Project Cost
+K. Project Details
+"</t>
+  </si>
+  <si>
+    <t>18P1415</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Proposed Development at Lot 286, Opposite Tabung Haji, KL
+B. Client
+Build King Construction Limited
+C. Type of Development
+-
+D. Geology Formation
+E. Land Area (acre)
+F. How Many Blocks &amp; Storeys
+G. Total Build-up Area (sq.m)
+H. Foundation System used
+I. Basement Levels &amp; Depth
+J. Estimated Total Project Cost
+K. Project Details
+"</t>
+  </si>
+  <si>
+    <t>18G1414</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Kepong Residence - Survey Plan &amp; KM Submission Layout
+B. Client
+G&amp;P Infra Sdn Bhd
+C. Type of Development
+Residential Condominium
+D. Geology Formation
+E. Land Area (acre)
+F. How Many Blocks &amp; Storeys
+G. Total Build-up Area (sq.m)
+H. Foundation System used
+I. Basement Levels &amp; Depth
+J. Estimated Total Project Cost
+K. Project Details
+"</t>
+  </si>
+  <si>
+    <t>18G1413</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Proposed Commercial Development for Mercedes Benz at Lot 168853, Bandar Parklands, Klang, Selangor
+B. Client
+Hap Seng Land Development (Puchong) Sdn Bhd
+C. Type of Development
+Commercial Development
+D. Geology Formation
+E. Land Area (acre)
+F. How Many Blocks &amp; Storeys
+G. Total Build-up Area (sq.m)
+H. Foundation System used
+I. Basement Levels &amp; Depth
+J. Estimated Total Project Cost
+K. Project Details
+"</t>
+  </si>
+  <si>
+    <t>18G1412-Marina, Petak 'C'</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Marina, Lot 15739, Mukim 12, Daerah Barat Daya, Penang
+B. Client
+Ideal Gim Venture Sdn Bhd
+C. Type of Development
+Marina
+D. Geology Formation
+E. Land Area (acre)
+F. How Many Blocks &amp; Storeys
+G. Total Build-up Area (sq.m)
+H. Foundation System used
+I. Basement Levels &amp; Depth
+J. Estimated Total Project Cost
+K. Project Details
+"</t>
+  </si>
+  <si>
+    <t>18G1411</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Phase 8, Jade Hills 
+B. Client
+G&amp;P Infra Sdn Bhd
+C. Type of Development
+-
+D. Geology Formation
+Kajang Formation 
+E. Land Area (acre)
+-
+F. How Many Blocks &amp; Storeys
+9 Blocks 2 Storeys
+G. Total Build-up Area (sq.m)
+-
+H. Foundation System used
+-
+I. Basement Levels &amp; Depth
+-
+J. Estimated Total Project Cost
+-
+K. Project Details
+Detailed SI &amp; Foundation Design"</t>
+  </si>
+  <si>
+    <t>18G1407</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Lot 30353, Jalan 34/26, Wangsa Maju, Setapak, KL - Full Geo
+B. Client
+Sunglobal Resources Sdn Bhd
+C. Type of Development
+Low Rise and High Rise
+D. Geology Formation
+Kenny Hill
+E. Land Area (acre)
+-
+F. How Many Blocks &amp; Storeys
+2 Blocks  
+G. Total Build-up Area (sq.m)
+-
+H. Foundation System used
+-
+I. Basement Levels &amp; Depth
+37 Levels
+J. Estimated Total Project Cost
+-
+K. Project Details
+Foundation and retaining wall"</t>
+  </si>
+  <si>
+    <t>18G1404</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Jade Hills Highzone and Road to Taman Sutera
+B. Client
+Jade Homes Sdn Bhd
+C. Type of Development
+Residential
+D. Geology Formation
+-
+E. Land Area (acre)
+44
+F. How Many Blocks &amp; Storeys
+-
+G. Total Build-up Area (sq.m)
+-
+H. Foundation System used
+-
+I. Basement Levels &amp; Depth
+-
+J. Estimated Total Project Cost
+-
+K. Project Details
+-"</t>
+  </si>
+  <si>
+    <t>18G1405</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+TNB Reserve at Northern Boundary of Jade Hills
+B. Client
+Jade Homes Sdn Bhd
+C. Type of Development
+-
+D. Geology Formation
+Kajang Formation 
+E. Land Area (acre)
+-
+F. How Many Blocks &amp; Storeys
+-
+G. Total Build-up Area (sq.m)
+-
+H. Foundation System used
+-
+I. Basement Levels &amp; Depth
+-
+J. Estimated Total Project Cost
+-
+K. Project Details
+Earthwork, CAT and FILL"</t>
+  </si>
+  <si>
+    <t>18G1406</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Setia Alam Sari Phase 9P1, 9P2, 9P4
+B. Client
+G&amp;P Infra Sdn Bhd
+C. Type of Development
+Housing Development
+D. Geology Formation
+Kajang Formation 
+E. Land Area (acre)
+-
+F. How Many Blocks &amp; Storeys
+2 Storeys
+G. Total Build-up Area (sq.m)
+-
+H. Foundation System used
+Driven RC / Spun Piles
+I. Basement Levels &amp; Depth
+-
+J. Estimated Total Project Cost
+-
+K. Project Details
+Foundation Design (RC Pile 150mm x 150m) pile length:12m @ 15m"</t>
+  </si>
+  <si>
+    <t>18G1396-LPT, OKP, JGB</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Proposed Butterworth Port, Penang 
+B. Client
+Ideal Gim Venture Sdn Bhd
+C. Type of Development
+Reclamation
+D. Geology Formation
+-
+E. Land Area (acre)
+217
+F. How Many Blocks &amp; Storeys
+-
+G. Total Build-up Area (sq.m)
+-
+H. Foundation System used
+-
+I. Basement Levels &amp; Depth
+-
+J. Estimated Total Project Cost
+-
+K. Project Details
+Prefabricated Veritical Drains (PVD), Surcharge, Embankments"</t>
+  </si>
+  <si>
+    <t>18E1391</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Sabah Sarawak Gas Pipeline - Gas Leak
+B. Client
+Petroliam Nasional Berhad (PETRONAS)
+C. Type of Development
+Forensil Investigation
+D. Geology Formation
+E. Land Area (acre)
+F. How Many Blocks &amp; Storeys
+G. Total Build-up Area (sq.m)
+H. Foundation System used
+I. Basement Levels &amp; Depth
+J. Estimated Total Project Cost
+K. Project Details
+"</t>
+  </si>
+  <si>
+    <t>18G1398</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Bandar Bukit Raja 2, R12A, R12B, R11A
+B. Client
+G&amp;P Infra Sdn Bhd
+C. Type of Development
+Low Rise
+D. Geology Formation
+Alluvium
+E. Land Area (acre)
+-
+F. How Many Blocks &amp; Storeys
+-
+G. Total Build-up Area (sq.m)
+-
+H. Foundation System used
+-
+I. Basement Levels &amp; Depth
+-
+J. Estimated Total Project Cost
+-
+K. Project Details
+Pile Strip Raft"</t>
+  </si>
+  <si>
+    <t>18G1403</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Melaka Refinery Diesel Euro 5 (MRDE5)
+B. Client
+Geolab (M) Sdn Bhd
+C. Type of Development
+Oil &amp; Gas
+D. Geology Formation
+-
+E. Land Area (acre)
+-
+F. How Many Blocks &amp; Storeys
+-
+G. Total Build-up Area (sq.m)
+-
+H. Foundation System used
+-
+I. Basement Levels &amp; Depth
+-
+J. Estimated Total Project Cost
+-
+K. Project Details
+Seismic Hazard Assessment by NGI"</t>
+  </si>
+  <si>
+    <t>18G1395</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Proposed Autohaus on Lot PT26923 (HS(D).283015), Mukim Bukit Raja
+B. Client
+Hap Seng Land Development (Puchong) Sdn Bhd
+C. Type of Development
+Commercial
+D. Geology Formation
+Kenny Hill
+E. Land Area (acre)
+1.8
+F. How Many Blocks &amp; Storeys
+10 Storeys
+G. Total Build-up Area (sq.m)
+-
+H. Foundation System used
+-
+I. Basement Levels &amp; Depth
+-
+J. Estimated Total Project Cost
+-
+K. Project Details
+Foundation (Piling)"</t>
+  </si>
+  <si>
+    <t>18G1402</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Knowledge Centre, Elmina West
+B. Client
+G&amp;P Infra Sdn Bhd
+C. Type of Development
+-
+D. Geology Formation
+Kenny Hill Foundation
+E. Land Area (acre)
+1.1
+F. How Many Blocks &amp; Storeys
+1 Block 1 Storey
+G. Total Build-up Area (sq.m)
+562m²
+H. Foundation System used
+Pad Footing
+I. Basement Levels &amp; Depth
+-
+J. Estimated Total Project Cost
+-
+K. Project Details
+Shallow Foundation"</t>
+  </si>
+  <si>
+    <t>18G1400</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Double Track Railway Project - Gemas to Kluang
+B. Client
+Sykt. Pemb. Yeoh Tiong Lay Sdn Bhd
+C. Type of Development
+Rail
+D. Geology Formation
+Alluvium &amp; Gemas / Semantan Foundation &amp; Segamat Basalt
+E. Land Area (acre)
+-
+F. How Many Blocks &amp; Storeys
+-
+G. Total Build-up Area (sq.m)
+-
+H. Foundation System used
+Bored Piles
+I. Basement Levels &amp; Depth
+-
+J. Estimated Total Project Cost
+-
+K. Project Details
+-"</t>
+  </si>
+  <si>
+    <t>18G1399</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Brogaville, Semenyih
+B. Client
+G&amp;P Infra Sdn Bhd
+C. Type of Development
+Low Rise
+D. Geology Formation
+Granite
+E. Land Area (acre)
+209
+F. How Many Blocks &amp; Storeys
+3 Blk Shoplot w 2 storeys, Bungalow &amp; Semi-D
+G. Total Build-up Area (sq.m)
+-
+H. Foundation System used
+Jack-in RC/Spun Piles
+I. Basement Levels &amp; Depth
+-
+J. Estimated Total Project Cost
+-
+K. Project Details
+RC Pile : (150mm SQ, 21m, 250kN), (200mm SQ, 21m, 450kN), (200mm Sq, 18m,450kN), (300mm SQ, 21m, 1000kN), (300mm SQ, 21m, 1000kN), RCW, RSW"</t>
+  </si>
+  <si>
+    <t>18E1389</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Smart Tunnel Maintenance Depot Office at Tun Razak Exchange
+B. Client
+TRX City Sdn Bhd
+C. Type of Development
+Low Rise Building
+D. Geology Formation
+KL Limestone
+E. Land Area (acre)
+-
+F. How Many Blocks &amp; Storeys
+3 Storeys
+G. Total Build-up Area (sq.m)
+-
+H. Foundation System used
+Micropiles
+I. Basement Levels &amp; Depth
+-
+J. Estimated Total Project Cost
+-
+K. Project Details
+Foundation &amp; Pile Load Test Review"</t>
+  </si>
+  <si>
+    <t>18G1401</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Glengowrie, Semenyih
+B. Client
+G&amp;P Infra Sdn Bhd
+C. Type of Development
+Hill Slope Development
+D. Geology Formation
+Granite
+E. Land Area (acre)
+800
+F. How Many Blocks &amp; Storeys
+-
+G. Total Build-up Area (sq.m)
+-
+H. Foundation System used
+-
+I. Basement Levels &amp; Depth
+-
+J. Estimated Total Project Cost
+-
+K. Project Details
+Retaining Wall System, Slope Strengthening System"</t>
+  </si>
+  <si>
+    <t>18G1392 Site Location</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Geotechnical and Traffic at San Peng Lot PT1052 (HSD115367) Seksyen 54, Kuala Lumpur
+B. Client
+LTS Skyline Sdn Bhd
+C. Type of Development
+-
+D. Geology Formation
+Limestone
+E. Land Area (acre)
+-
+F. How Many Blocks &amp; Storeys
+-
+G. Total Build-up Area (sq.m)
+-
+H. Foundation System used
+Bored Piles
+I. Basement Levels &amp; Depth
+-
+J. Estimated Total Project Cost
+-
+K. Project Details
+Foundation and Retaining Wall"</t>
+  </si>
+  <si>
+    <t>18G1393</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Proposed Bridge at One Foresta Development, Bayan Lepas, Penang
+B. Client
+Ideal Property Development Sdn Bhd
+C. Type of Development
+Mix Development
+D. Geology Formation
+Tanjung Bunga Granite
+E. Land Area (acre)
+-
+F. How Many Blocks &amp; Storeys
+-
+G. Total Build-up Area (sq.m)
+-
+H. Foundation System used
+-
+I. Basement Levels &amp; Depth
+-
+J. Estimated Total Project Cost
+-
+K. Project Details
+Soil Nail (32mm diameter &amp; 15m length)"</t>
+  </si>
+  <si>
+    <t>18E1394</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Tapah Plant, Perak
+B. Client
+Lhoist (Malaysia) Sdn Bhd
+C. Type of Development
+Quarry
+D. Geology Formation
+Limestone
+E. Land Area (acre)
+-
+F. How Many Blocks &amp; Storeys
+-
+G. Total Build-up Area (sq.m)
+-
+H. Foundation System used
+-
+I. Basement Levels &amp; Depth
+-
+J. Estimated Total Project Cost
+-
+K. Project Details
+Expert Review"</t>
+  </si>
+  <si>
+    <t>18F1390-Pejabat Pentadbiran SKVE</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+South Klang Valley Expressway (SKVE)
+B. Client
+PLUS Malaysia Berhad
+C. Type of Development
+-
+D. Geology Formation
+Alluvium
+E. Land Area (acre)
+-
+F. How Many Blocks &amp; Storeys
+-
+G. Total Build-up Area (sq.m)
+-
+H. Foundation System used
+Driven RC / Spun Piles
+I. Basement Levels &amp; Depth
+-
+J. Estimated Total Project Cost
+-
+K. Project Details
+-"</t>
+  </si>
+  <si>
+    <t>18G1397</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+New Mine Pit Design, Pengkalan Hulu, Perak
+B. Client
+Rahman Hydraulic Tin Sdn Bhd
+C. Type of Development
+-
+D. Geology Formation
+Sedimentosy - pyrodastic Sequence
+E. Land Area (acre)
+-
+F. How Many Blocks &amp; Storeys
+-
+G. Total Build-up Area (sq.m)
+-
+H. Foundation System used
+-
+I. Basement Levels &amp; Depth
+-
+J. Estimated Total Project Cost
+-
+K. Project Details
+Design of soil &amp; rod slope for about 200m deep open excavation for mining "</t>
+  </si>
+  <si>
+    <t>18A1410</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Warehouse for IKEA, Pulau Indah
+B. Client
+Keller (M) Sdn Bhd
+C. Type of Development
+Commercial
+D. Geology Formation
+E. Land Area (acre)
+F. How Many Blocks &amp; Storeys
+G. Total Build-up Area (sq.m)
+H. Foundation System used
+I. Basement Levels &amp; Depth
+J. Estimated Total Project Cost
+K. Project Details
+"</t>
+  </si>
+  <si>
+    <t>18G1409</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Culvert Crossing at Lingkaran Cassia Barat, Batu Kawan, Pulau Pinang
+B. Client
+Penang Development Corporation
+C. Type of Development
+Infrastructure (Foundation of Culvert)
+D. Geology Formation
+Alluvium
+E. Land Area (acre)
+-
+F. How Many Blocks &amp; Storeys
+-
+G. Total Build-up Area (sq.m)
+-
+H. Foundation System used
+Culvert's Foundation &amp; Structure Design
+I. Basement Levels &amp; Depth
+-
+J. Estimated Total Project Cost
+-
+K. Project Details
+Foundation &amp; Structure design for culvert on trated area"</t>
+  </si>
+  <si>
+    <t>18G1408</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+EDIS Earth Work with Soil Treatment at Batu Kawan, Pulau Pinang (PITP) (16.72 acres)
+B. Client
+Penang Development Corporation
+C. Type of Development
+Highrise Building
+D. Geology Formation
+Limestone
+E. Land Area (acre)
+4.4
+F. How Many Blocks &amp; Storeys
+2 Blocks 45 Storeys
+G. Total Build-up Area (sq.m)
+-
+H. Foundation System used
+-
+I. Basement Levels &amp; Depth
+1 Sub Basement
+J. Estimated Total Project Cost
+-
+K. Project Details
+Foundation &amp; Cavity Treatment"
+I. Basement Levels &amp; Depth
+J. Estimated Total Project Cost
+K. Project Details
+"</t>
+  </si>
+  <si>
+    <t>18E1416</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Proposed Industrial Development at Shah Alam
+B. Client
+Nakano Construction Sdn Bhd
+C. Type of Development
+Industrial Development
+D. Geology Formation
+Kenny Hill Formation
+E. Land Area (acre)
+20.2
+F. How Many Blocks &amp; Storeys
+-
+G. Total Build-up Area (sq.m)
+12.5
+H. Foundation System used
+-
+I. Basement Levels &amp; Depth
+1 Basement 6m depth
+J. Estimated Total Project Cost
+400 million
+K. Project Details
+Piles Issues during Construction Period"</t>
+  </si>
+  <si>
+    <t>18G1417</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Setia Ecohill 2
+B. Client
+G&amp;P Infra Sdn Bhd
+C. Type of Development
+Mixed Housing Development &amp; Business
+D. Geology Formation
+Jelebu Schist Formation and at Contact Boundary of Granite Formatic
+E. Land Area (acre)
+-
+F. How Many Blocks &amp; Storeys
+-
+G. Total Build-up Area (sq.m)
+-
+H. Foundation System used
+-
+I. Basement Levels &amp; Depth
+-
+J. Estimated Total Project Cost
+-
+K. Project Details
+Detailed SI Subsurface Investigation"</t>
+  </si>
+  <si>
+    <t>18F1438</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Proposed Industrial Developments At Ipark, Sac, Mukim Terbau, Daerah Johor Bahru
+B. Client
+Senai Airport City Sdn Bhd
+C. Type of Development
+Industrial
+D. Geology Formation
+Granite Formation
+E. Land Area (acre)
+140
+F. How Many Blocks &amp; Storeys
+2 Storeys Factories
+G. Total Build-up Area (sq.m)
+-
+H. Foundation System used
+-
+I. Basement Levels &amp; Depth
+-
+J. Estimated Total Project Cost
+-
+K. Project Details
+Forensic SI, electrical resistivity survey"</t>
+  </si>
+  <si>
+    <t>18G1437</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Proposed 20MW Solar PV Project At Plot 11, A Portion of Lot 5 (Approx 72 Acres), Pekan Bukit Selambau, Daerah Kuala Muda, Kedah
+B. Client
+G&amp;P Infra Sdn Bhd
+C. Type of Development
+D. Geology Formation
+E. Land Area (acre)
+F. How Many Blocks &amp; Storeys
+G. Total Build-up Area (sq.m)
+H. Foundation System used
+I. Basement Levels &amp; Depth
+J. Estimated Total Project Cost
+K. Project Details
+"</t>
+  </si>
+  <si>
+    <t>18G1436</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Proposed Development At Bandar Sri Ehsan (1200 Acres), Sepang, Selangor
+B. Client
+Brunsfield Engineering Sdn Bhd
+C. Type of Development
+D. Geology Formation
+E. Land Area (acre)
+F. How Many Blocks &amp; Storeys
+G. Total Build-up Area (sq.m)
+H. Foundation System used
+I. Basement Levels &amp; Depth
+J. Estimated Total Project Cost
+K. Project Details
+"</t>
+  </si>
+  <si>
+    <t>18E1427</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Earthwork Planning for Access Road Construction Point D for Hyper Act Marketing
+B. Client
+Hyper Act Marketing Sdn Bhd
+C. Type of Development
+Quarry Site
+D. Geology Formation
+Limestone
+E. Land Area (acre)
+103.02
+F. How Many Blocks &amp; Storeys
+-
+G. Total Build-up Area (sq.m)
+-
+H. Foundation System used
+-
+I. Basement Levels &amp; Depth
+-
+J. Estimated Total Project Cost
+39696268.8
+K. Project Details
+Earthwork Planning"</t>
+  </si>
+  <si>
+    <t>18E1428</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Proposed Design &amp; Build for Jalan Tg Kupang, Gerbang Nusajaya and New Interghange including New Slip Road from PLUS Second Link Highway
+B. Client
+Nusajaya Rise Sdn Bhd
+C. Type of Development
+Infrastructure
+D. Geology Formation
+Jurong Formation
+E. Land Area (acre)
+-
+F. How Many Blocks &amp; Storeys
+-
+G. Total Build-up Area (sq.m)
+-
+H. Foundation System used
+-
+I. Basement Levels &amp; Depth
+-
+J. Estimated Total Project Cost
+-
+K. Project Details
+-"</t>
+  </si>
+  <si>
+    <t>18M1429</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+In The Matter Of Arbitration Between UEM Builders &amp; Edgenta Propel (Claimants) And Ocned Water Technology (Respondent)
+B. Client
+Ocned Water Technolgy Sdn Bhd
+C. Type of Development
+-
+D. Geology Formation
+-
+E. Land Area (acre)
+-
+F. How Many Blocks &amp; Storeys
+-
+G. Total Build-up Area (sq.m)
+-
+H. Foundation System used
+-
+I. Basement Levels &amp; Depth
+-
+J. Estimated Total Project Cost
+25300000
+K. Project Details
+-"</t>
+  </si>
+  <si>
+    <t>18P1430</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Wind Farm In India 
+B. Client
+Adani Wind Energy Guj Pvt Ltd
+C. Type of Development
+-
+D. Geology Formation
+Alluvium, Rann Sand (Quarternary Deposits)
+E. Land Area (acre)
+-
+F. How Many Blocks &amp; Storeys
+-
+G. Total Build-up Area (sq.m)
+-
+H. Foundation System used
+-
+I. Basement Levels &amp; Depth
+-
+J. Estimated Total Project Cost
+-
+K. Project Details
+1 Wind Turbine At 2 Borehole Location"</t>
+  </si>
+  <si>
+    <t>18G1418</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Inspection of Swimming Pool at PV10 Platinum Lake Condominium, Setapak, Kuala Lumpur
+B. Client
+PV10 Management Corporation
+C. Type of Development
+-
+D. Geology Formation
+-
+E. Land Area (acre)
+-
+F. How Many Blocks &amp; Storeys
+-
+G. Total Build-up Area (sq.m)
+-
+H. Foundation System used
+-
+I. Basement Levels &amp; Depth
+-
+J. Estimated Total Project Cost
+-
+K. Project Details
+Swimming Pool Imspection"</t>
+  </si>
+  <si>
+    <t>18E1423</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Sunway Medical Centre, Seberang Jaya, Pulau Pinang
+B. Client
+Alliance Parade Sdn Bhd
+C. Type of Development
+-
+D. Geology Formation
+Clay / Silt
+E. Land Area (acre)
+11.13
+F. How Many Blocks &amp; Storeys
+1 Block &amp; 9 Storeys
+G. Total Build-up Area (sq.m)
+-
+H. Foundation System used
+-
+I. Basement Levels &amp; Depth
+1 basement 6.8m depth
+J. Estimated Total Project Cost
+-
+K. Project Details
+Jack In Pile - 48m to 60m length, 500mm Dia spun pile"</t>
+  </si>
+  <si>
+    <t>18F1424</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Hyper Act Marketing (akta HAM) Blasting Incident
+B. Client
+Hyper Act Marketing Sdn Bhd
+C. Type of Development
+-
+D. Geology Formation
+Limestone
+E. Land Area (acre)
+103.02
+F. How Many Blocks &amp; Storeys
+-
+G. Total Build-up Area (sq.m)
+-
+H. Foundation System used
+-
+I. Basement Levels &amp; Depth
+-
+J. Estimated Total Project Cost
+-
+K. Project Details
+Forensic Investigation"</t>
+  </si>
+  <si>
+    <t>18M1425</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Tilted House at No.6 Jln Impian 10B/KS7, Bdr Botanic, Klang (PH30)
+B. Client
+Gamuda Land (Botanic) Sdn Bhd
+C. Type of Development
+-
+D. Geology Formation
+Soft Clay
+E. Land Area (acre)
+-
+F. How Many Blocks &amp; Storeys
+-
+G. Total Build-up Area (sq.m)
+-
+H. Foundation System used
+-
+I. Basement Levels &amp; Depth
+-
+J. Estimated Total Project Cost
+-
+K. Project Details
+Arbitration &amp; Mediation"</t>
+  </si>
+  <si>
+    <t>18G1421</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Proposed Development Site 2 - Extension Of 3S CV &amp; 1S PC Facilities Including Carparks  To Existing Ccb Mercedes Benz Showroom At Jalan Perusahaan Satu/Dua, Batu Cave, Kuala Lumpur
+B. Client
+Savills (Project Management) Sdn Bhd
+C. Type of Development
+-
+D. Geology Formation
+Limestone
+E. Land Area (acre)
+-
+F. How Many Blocks &amp; Storeys
+1 Carpark
+G. Total Build-up Area (sq.m)
+-
+H. Foundation System used
+-
+I. Basement Levels &amp; Depth
+-
+J. Estimated Total Project Cost
+-
+K. Project Details
+Piling    "</t>
+  </si>
+  <si>
+    <t>18P1422</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Puncak Alam (MKH)
+B. Client
+G&amp;P Infra Sdn Bhd
+C. Type of Development
+-
+D. Geology Formation
+Kenny Hill
+E. Land Area (acre)
+-
+F. How Many Blocks &amp; Storeys
+-
+G. Total Build-up Area (sq.m)
+-
+H. Foundation System used
+-
+I. Basement Levels &amp; Depth
+-
+J. Estimated Total Project Cost
+-
+K. Project Details
+-"</t>
+  </si>
+  <si>
+    <t>18P1431</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Hyper Act Marketing (akta HAM) Blasting Incident
+B. Client
+Hyper Act Marketing Sdn Bhd
+C. Type of Development
+-
+D. Geology Formation
+Limestone
+E. Land Area (acre)
+103.02
+F. How Many Blocks &amp; Storeys
+-
+G. Total Build-up Area (sq.m)
+-
+H. Foundation System used
+-
+I. Basement Levels &amp; Depth
+-
+J. Estimated Total Project Cost
+1617768.1
+K. Project Details
+-"</t>
+  </si>
+  <si>
+    <t>18G1432</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Sunway Medical Centre @ Damansara
+B. Client
+Sunway Integrated Properties Sdn Bhd
+C. Type of Development
+-
+D. Geology Formation
+Granite
+E. Land Area (acre)
+2.33
+F. How Many Blocks &amp; Storeys
+1 Block 13 Levels
+G. Total Build-up Area (sq.m)
+88558
+H. Foundation System used
+-
+I. Basement Levels &amp; Depth
+2 Basements
+J. Estimated Total Project Cost
+-
+K. Project Details
+Foundation &amp; Temporary Sheatpile Wall"</t>
+  </si>
+  <si>
+    <t>18E1433</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Foundation Review at Taman Kuchai Jaya
+B. Client
+Menta Land Sdn Bhd
+C. Type of Development
+Highrise, Residential Develpoment &amp; Commercial
+D. Geology Formation
+Granitic, contact boundary with Kenny Hill
+E. Land Area (acre)
+-
+F. How Many Blocks &amp; Storeys
+-
+G. Total Build-up Area (sq.m)
+-
+H. Foundation System used
+-
+I. Basement Levels &amp; Depth
+-
+J. Estimated Total Project Cost
+-
+K. Project Details
+Foundation Review at Taman Kuchai Jaya"</t>
+  </si>
+  <si>
+    <t>18F1434</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Ground Settlement Around 19 Units Of Terrace Houses At Bandar Bukit Raja I, Phase 15 (Nahara)
+B. Client
+Sime Darby USJ Development Sdn Bhd
+C. Type of Development
+-
+D. Geology Formation
+Clay 
+E. Land Area (acre)
+-
+F. How Many Blocks &amp; Storeys
+-
+G. Total Build-up Area (sq.m)
+-
+H. Foundation System used
+-
+I. Basement Levels &amp; Depth
+-
+J. Estimated Total Project Cost
+-
+K. Project Details
+Investigate on ground settlement"</t>
+  </si>
+  <si>
+    <t>18G1435</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Solaris PARQ Plot B
+B. Client
+UEM Sunrise Berhad
+C. Type of Development
+Mixed
+D. Geology Formation
+Metasedimentary
+E. Land Area (acre)
+12.56
+F. How Many Blocks &amp; Storeys
+50 storeys
+G. Total Build-up Area (sq.m)
+50823
+H. Foundation System used
+-
+I. Basement Levels &amp; Depth
+9 Sub Basement, 31.2m (max)
+J. Estimated Total Project Cost
+-
+K. Project Details
+Retaining System &amp; Foundation"</t>
+  </si>
+  <si>
+    <t>18P1440</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Mixed Development on 3 acres on Lot 20087 at Ujung Batu, Jalan Bagan Dalam, Seksyen 4, Seberang Perai Utara, Pulau Pinang
+B. Client
+Perbadanan Pembangunan Pulau Pinang (Penang Dev. Corp)
+C. Type of Development
+D. Geology Formation
+E. Land Area (acre)
+F. How Many Blocks &amp; Storeys
+G. Total Build-up Area (sq.m)
+H. Foundation System used
+I. Basement Levels &amp; Depth
+J. Estimated Total Project Cost
+K. Project Details
+"</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+L3A Bukit Jelutong, Shah Alam
+B. Client
+G&amp;P Infra Sdn Bhd
+C. Type of Development
+D. Geology Formation
+E. Land Area (acre)
+F. How Many Blocks &amp; Storeys
+G. Total Build-up Area (sq.m)
+H. Foundation System used
+I. Basement Levels &amp; Depth
+J. Estimated Total Project Cost
+K. Project Details
+"</t>
+  </si>
+  <si>
+    <t>"18G1407
+A. Project Tittle
+Lot 30353, Jalan 34/26, Wangsa Maju, Setapak, KL - Full Geo
+B. Client
+Sunglobal Resources Sdn Bhd
+C. Type of Development
+Low Rise and High Rise
+D. Geology Formation
+Kenny Hill
+E. Land Area (acre)
+-
+F. How Many Blocks &amp; Storeys
+-
+G. Total Build-up Area (sq.m)
+-
+H. Foundation System used
+-
+I. Basement Levels &amp; Depth
+-
+J. Estimated Total Project Cost
+-
+K. Project Details
+Foundation and retaining wall"</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Jade Hills Highzone and Road to Taman Sutera
+B. Client
+Jade Homes Sdn Bhd
+C. Type of Development
+Residential
+D. Geology Formation
+Kajang Formation 
+E. Land Area (acre)
+44
+F. How Many Blocks &amp; Storeys
+-
+G. Total Build-up Area (sq.m)
+-
+H. Foundation System used
+-
+I. Basement Levels &amp; Depth
+-
+J. Estimated Total Project Cost
+-
+K. Project Details
+-"</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Setia Alam Sari Phase 9P1, 9P2, 9P4
+B. Client
+G&amp;P Infra Sdn Bhd
+C. Type of Development
+Housing Development
+D. Geology Formation
+Kajang Formation 
+E. Land Area (acre)
+-
+F. How Many Blocks &amp; Storeys
+2 Storeys
+G. Total Build-up Area (sq.m)
+-
+H. Foundation System used
+Driven RC / Spun Piles
+I. Basement Levels &amp; Depth
+-
+J. Estimated Total Project Cost
+-
+K. Project Details
+Foundation Design (RC Pile 175mm x 175m) pile length:15m"</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Proposed Autohaus on Lot PT26923 (HS(D).283015), Mukim Bukit Raja
+B. Client
+Hap Seng Land Development (Puchong) Sdn Bhd
+C. Type of Development
+Commercial
+D. Geology Formation
+Kenny Hill
+E. Land Area (acre)
+1.8
+F. How Many Blocks &amp; Storeys
+-
+G. Total Build-up Area (sq.m)
+-
+H. Foundation System used
+-
+I. Basement Levels &amp; Depth
+-
+J. Estimated Total Project Cost
+-
+K. Project Details
+Foundation (Piling)"</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Brogaville, Semenyih
+B. Client
+G&amp;P Infra Sdn Bhd
+C. Type of Development
+Low Rise
+D. Geology Formation
+Granite
+E. Land Area (acre)
+209
+F. How Many Blocks &amp; Storeys
+3 Blk Shoplot w 2 storeys, Bungalow &amp; Semi-D
+G. Total Build-up Area (sq.m)
+-
+H. Foundation System used
+Jack-in RC/Spun Piles
+I. Basement Levels &amp; Depth
+-
+J. Estimated Total Project Cost
+-
+K. Project Details
+Spun Pile &amp; Retaining Wall"</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Proposed Industrial Developments At Ipark, Sac, Mukim Terbau, Daerah Johor Bahru
+B. Client
+Senai Airport City Sdn Bhd
+C. Type of Development
+Industrial
+D. Geology Formation
+Granite Formation
+E. Land Area (acre)
+Approx 140
+F. How Many Blocks &amp; Storeys
+2 Storeys Factories
+G. Total Build-up Area (sq.m)
+-
+H. Foundation System used
+-
+I. Basement Levels &amp; Depth
+-
+J. Estimated Total Project Cost
+-
+K. Project Details
+Forensic SI, resistivity"</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Proposed 20MW Solar PV Project At Plot 11, A Portion of Lot 5 (Approx 72 Acres), Pekan Bukit Selambau, Daerah Kuala Muda, Kedah
+B. Client
+G&amp;P Infra Sdn Bhd
+C. Type of Development
+Industrial
+D. Geology Formation
+-
+E. Land Area (acre)
+72
+F. How Many Blocks &amp; Storeys
+-
+G. Total Build-up Area (sq.m)
+-
+H. Foundation System used
+-
+I. Basement Levels &amp; Depth
+-
+J. Estimated Total Project Cost
+-
+K. Project Details
+Retaining Wall and Formation"</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Hyper Act Marketing (akta HAM) Blasting Incident
+B. Client
+Hyper Act Marketing Sdn Bhd
+C. Type of Development
+-
+D. Geology Formation
+Limestone
+E. Land Area (acre)
+-
+F. How Many Blocks &amp; Storeys
+-
+G. Total Build-up Area (sq.m)
+-
+H. Foundation System used
+-
+I. Basement Levels &amp; Depth
+-
+J. Estimated Total Project Cost
+-
+K. Project Details
+Forensic Investigation"</t>
+  </si>
+  <si>
+    <t>18G1420</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Proposed Development On Site 1 - Ccb Mercedes Benz 3-S Showroom &amp; Facilities At Lot 338, Jalan Sungai Besi 
+B. Client
+Savills (Project Management) Sdn Bhd
+C. Type of Development
+Commercial
+D. Geology Formation
+Limestone
+E. Land Area (acre)
+1.05
+F. How Many Blocks &amp; Storeys
+1 block &amp; 9 storey
+G. Total Build-up Area (sq.m)
+-
+H. Foundation System used
+-
+I. Basement Levels &amp; Depth
+-
+J. Estimated Total Project Cost
+-
+K. Project Details
+Bored pile (BP 1000, 1350, 1200, 1500, 2000). Ave pile length 5m + rock socket"</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Mixed Development on 3 acres on Lot 20087 at Ujung Batu, Jalan Bagan Dalam, Seksyen 4, Seberang Perai Utara, Pulau Pinang
+B. Client
+Perbadanan Pembangunan Pulau Pinang (Penang Dev. Corp)
+C. Type of Development
+-
+D. Geology Formation
+Alluvium Formation
+E. Land Area (acre)
+-
+F. How Many Blocks &amp; Storeys
+-
+G. Total Build-up Area (sq.m)
+-
+H. Foundation System used
+-
+I. Basement Levels &amp; Depth
+-
+J. Estimated Total Project Cost
+-
+K. Project Details
+Soft Ground Engineering and Ground Treatment"</t>
+  </si>
+  <si>
+    <t>A. Project Tittle
+Solaris PARQ Plot B
+B. Client
+UEM Sunrise Berhad
+C. Type of Development
+D. Geology Formation
+E. Land Area (acre)
+F. How Many Blocks &amp; Storeys
+G. Total Build-up Area (sq.m)
+H. Foundation System used
+I. Basement Levels &amp; Depth
+J. Estimated Total Project Cost
+K. Project Details
+"</t>
   </si>
 </sst>
 </file>
@@ -26512,8 +28121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7097F85E-58BC-4772-9C3D-A515B54ADF6E}">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -27409,12 +29018,3279 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B76E8AB-8CDF-4DA9-AF3F-77B35D070432}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E192"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>101.882469444444</v>
+      </c>
+      <c r="B2">
+        <v>3.0769194444444401</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1604</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1605</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>101.522327777778</v>
+      </c>
+      <c r="B3">
+        <v>3.1162416666666699</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1608</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1609</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>101.88246807070701</v>
+      </c>
+      <c r="B4">
+        <v>3.0769181002211701</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1604</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1610</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>101.721318173211</v>
+      </c>
+      <c r="B5">
+        <v>3.1579250000000001</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1611</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1612</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>101.642388888889</v>
+      </c>
+      <c r="B6">
+        <v>3.2101944444444399</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1613</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>101.46099080969699</v>
+      </c>
+      <c r="B7">
+        <v>2.9708643830146801</v>
+      </c>
+      <c r="C7">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1615</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1616</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>100.31079888201999</v>
+      </c>
+      <c r="B8">
+        <v>5.3321057681908304</v>
+      </c>
+      <c r="C8">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1617</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1618</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>101.754221851107</v>
+      </c>
+      <c r="B9">
+        <v>2.9988599116086299</v>
+      </c>
+      <c r="C9">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1619</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>101.736906173387</v>
+      </c>
+      <c r="B10">
+        <v>3.19259166666667</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1621</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1622</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>101.755873700831</v>
+      </c>
+      <c r="B11">
+        <v>2.9960222004371899</v>
+      </c>
+      <c r="C11">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1623</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1624</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>101.755816414771</v>
+      </c>
+      <c r="B12">
+        <v>3.00176388888889</v>
+      </c>
+      <c r="C12">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1625</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1626</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>101.79734166666699</v>
+      </c>
+      <c r="B13">
+        <v>2.9211555555555599</v>
+      </c>
+      <c r="C13">
+        <v>13</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1627</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1628</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>100.371392952373</v>
+      </c>
+      <c r="B14">
+        <v>5.4312633333092997</v>
+      </c>
+      <c r="C14">
+        <v>14</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1629</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1628</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>115.495166666667</v>
+      </c>
+      <c r="B15">
+        <v>4.28508333333333</v>
+      </c>
+      <c r="C15">
+        <v>15</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1631</v>
+      </c>
+      <c r="E15" t="s">
+        <v>1632</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>101.413580006853</v>
+      </c>
+      <c r="B16">
+        <v>3.1027349075927102</v>
+      </c>
+      <c r="C16">
+        <v>16</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1633</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1634</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>102.135175599516</v>
+      </c>
+      <c r="B17">
+        <v>2.2753854774955098</v>
+      </c>
+      <c r="C17">
+        <v>17</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1635</v>
+      </c>
+      <c r="E17" t="s">
+        <v>1636</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>101.448710529566</v>
+      </c>
+      <c r="B18">
+        <v>3.1094766836751</v>
+      </c>
+      <c r="C18">
+        <v>18</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1637</v>
+      </c>
+      <c r="E18" t="s">
+        <v>1638</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>101.500553540545</v>
+      </c>
+      <c r="B19">
+        <v>3.1711628199886901</v>
+      </c>
+      <c r="C19">
+        <v>19</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1639</v>
+      </c>
+      <c r="E19" t="s">
+        <v>1640</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>103.31847500000001</v>
+      </c>
+      <c r="B20">
+        <v>2.03000277777778</v>
+      </c>
+      <c r="C20">
+        <v>20</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1641</v>
+      </c>
+      <c r="E20" t="s">
+        <v>1642</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>101.87005609469701</v>
+      </c>
+      <c r="B21">
+        <v>2.9431088301614801</v>
+      </c>
+      <c r="C21">
+        <v>21</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1643</v>
+      </c>
+      <c r="E21" t="s">
+        <v>1644</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>101.718620000006</v>
+      </c>
+      <c r="B22">
+        <v>3.1400799999937501</v>
+      </c>
+      <c r="C22">
+        <v>22</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1645</v>
+      </c>
+      <c r="E22" t="s">
+        <v>1646</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>101.88354722222201</v>
+      </c>
+      <c r="B23">
+        <v>2.9099916666666701</v>
+      </c>
+      <c r="C23">
+        <v>23</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1647</v>
+      </c>
+      <c r="E23" t="s">
+        <v>1648</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>101.71223580399401</v>
+      </c>
+      <c r="B24">
+        <v>3.1339689441857601</v>
+      </c>
+      <c r="C24">
+        <v>24</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1649</v>
+      </c>
+      <c r="E24" t="s">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>100.256471874721</v>
+      </c>
+      <c r="B25">
+        <v>5.3001549762561204</v>
+      </c>
+      <c r="C25">
+        <v>25</v>
+      </c>
+      <c r="D25" t="s">
+        <v>1651</v>
+      </c>
+      <c r="E25" t="s">
+        <v>1652</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>101.19647543137501</v>
+      </c>
+      <c r="B26">
+        <v>4.2053316880020297</v>
+      </c>
+      <c r="C26">
+        <v>26</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1653</v>
+      </c>
+      <c r="E26" t="s">
+        <v>1654</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>101.52394700000001</v>
+      </c>
+      <c r="B27">
+        <v>2.914018</v>
+      </c>
+      <c r="C27">
+        <v>27</v>
+      </c>
+      <c r="D27" t="s">
+        <v>1655</v>
+      </c>
+      <c r="E27" t="s">
+        <v>1656</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>101.035922222222</v>
+      </c>
+      <c r="B28">
+        <v>5.5253361111111099</v>
+      </c>
+      <c r="C28">
+        <v>28</v>
+      </c>
+      <c r="D28" t="s">
+        <v>1657</v>
+      </c>
+      <c r="E28" t="s">
+        <v>1658</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>101.362702777778</v>
+      </c>
+      <c r="B29">
+        <v>2.9742999999999999</v>
+      </c>
+      <c r="C29">
+        <v>29</v>
+      </c>
+      <c r="D29" t="s">
+        <v>1659</v>
+      </c>
+      <c r="E29" t="s">
+        <v>1660</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>100.431811111111</v>
+      </c>
+      <c r="B30">
+        <v>5.2386111111111102</v>
+      </c>
+      <c r="C30">
+        <v>30</v>
+      </c>
+      <c r="D30" t="s">
+        <v>1661</v>
+      </c>
+      <c r="E30" t="s">
+        <v>1662</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>101.654180555556</v>
+      </c>
+      <c r="B31">
+        <v>3.2244555555555601</v>
+      </c>
+      <c r="C31">
+        <v>31</v>
+      </c>
+      <c r="D31" t="s">
+        <v>1663</v>
+      </c>
+      <c r="E31" t="s">
+        <v>1664</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>101.542266666667</v>
+      </c>
+      <c r="B32">
+        <v>3.0509972222222199</v>
+      </c>
+      <c r="C32">
+        <v>32</v>
+      </c>
+      <c r="D32" t="s">
+        <v>1665</v>
+      </c>
+      <c r="E32" t="s">
+        <v>1666</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>101.849952777778</v>
+      </c>
+      <c r="B33">
+        <v>2.8932222222222199</v>
+      </c>
+      <c r="C33">
+        <v>33</v>
+      </c>
+      <c r="D33" t="s">
+        <v>1667</v>
+      </c>
+      <c r="E33" t="s">
+        <v>1668</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>103.68018333333301</v>
+      </c>
+      <c r="B34">
+        <v>1.59805</v>
+      </c>
+      <c r="C34">
+        <v>34</v>
+      </c>
+      <c r="D34" t="s">
+        <v>1669</v>
+      </c>
+      <c r="E34" t="s">
+        <v>1670</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>100.613616666667</v>
+      </c>
+      <c r="B35">
+        <v>5.6596055555555598</v>
+      </c>
+      <c r="C35">
+        <v>35</v>
+      </c>
+      <c r="D35" t="s">
+        <v>1671</v>
+      </c>
+      <c r="E35" t="s">
+        <v>1672</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>101.62524444444399</v>
+      </c>
+      <c r="B36">
+        <v>2.76979166666667</v>
+      </c>
+      <c r="C36">
+        <v>36</v>
+      </c>
+      <c r="D36" t="s">
+        <v>1673</v>
+      </c>
+      <c r="E36" t="s">
+        <v>1674</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>101.154016666667</v>
+      </c>
+      <c r="B37">
+        <v>4.5289805555555596</v>
+      </c>
+      <c r="C37">
+        <v>37</v>
+      </c>
+      <c r="D37" t="s">
+        <v>1675</v>
+      </c>
+      <c r="E37" t="s">
+        <v>1676</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>103.590858333333</v>
+      </c>
+      <c r="B38">
+        <v>1.43166666666667</v>
+      </c>
+      <c r="C38">
+        <v>38</v>
+      </c>
+      <c r="D38" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E38" t="s">
+        <v>1678</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>104.111111111111</v>
+      </c>
+      <c r="B39">
+        <v>1.36470277777778</v>
+      </c>
+      <c r="C39">
+        <v>39</v>
+      </c>
+      <c r="D39" t="s">
+        <v>1679</v>
+      </c>
+      <c r="E39" t="s">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>69.569105555555595</v>
+      </c>
+      <c r="B40">
+        <v>24.0290416666667</v>
+      </c>
+      <c r="C40">
+        <v>40</v>
+      </c>
+      <c r="D40" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E40" t="s">
+        <v>1682</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>101.715363888889</v>
+      </c>
+      <c r="B41">
+        <v>3.2033083333333301</v>
+      </c>
+      <c r="C41">
+        <v>41</v>
+      </c>
+      <c r="D41" t="s">
+        <v>1683</v>
+      </c>
+      <c r="E41" t="s">
+        <v>1684</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>100.396916666667</v>
+      </c>
+      <c r="B42">
+        <v>5.3953527777777799</v>
+      </c>
+      <c r="C42">
+        <v>42</v>
+      </c>
+      <c r="D42" t="s">
+        <v>1685</v>
+      </c>
+      <c r="E42" t="s">
+        <v>1686</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>101.154016666667</v>
+      </c>
+      <c r="B43">
+        <v>4.5289805555555596</v>
+      </c>
+      <c r="C43">
+        <v>43</v>
+      </c>
+      <c r="D43" t="s">
+        <v>1687</v>
+      </c>
+      <c r="E43" t="s">
+        <v>1688</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>101.461252777778</v>
+      </c>
+      <c r="B44">
+        <v>2.9946305555555601</v>
+      </c>
+      <c r="C44">
+        <v>44</v>
+      </c>
+      <c r="D44" t="s">
+        <v>1689</v>
+      </c>
+      <c r="E44" t="s">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>101.68220833333299</v>
+      </c>
+      <c r="B45">
+        <v>3.2318833333333301</v>
+      </c>
+      <c r="C45">
+        <v>45</v>
+      </c>
+      <c r="D45" t="s">
+        <v>1691</v>
+      </c>
+      <c r="E45" t="s">
+        <v>1692</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>101.436333333333</v>
+      </c>
+      <c r="B46">
+        <v>3.2354972222222198</v>
+      </c>
+      <c r="C46">
+        <v>46</v>
+      </c>
+      <c r="D46" t="s">
+        <v>1693</v>
+      </c>
+      <c r="E46" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>101.154016666667</v>
+      </c>
+      <c r="B47">
+        <v>4.5289805555555596</v>
+      </c>
+      <c r="C47">
+        <v>47</v>
+      </c>
+      <c r="D47" t="s">
+        <v>1695</v>
+      </c>
+      <c r="E47" t="s">
+        <v>1696</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>101.59655833333299</v>
+      </c>
+      <c r="B48">
+        <v>3.1501027777777799</v>
+      </c>
+      <c r="C48">
+        <v>48</v>
+      </c>
+      <c r="D48" t="s">
+        <v>1697</v>
+      </c>
+      <c r="E48" t="s">
+        <v>1698</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>101.68445</v>
+      </c>
+      <c r="B49">
+        <v>3.0896055555555599</v>
+      </c>
+      <c r="C49">
+        <v>49</v>
+      </c>
+      <c r="D49" t="s">
+        <v>1699</v>
+      </c>
+      <c r="E49" t="s">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>101.45906388888901</v>
+      </c>
+      <c r="B50">
+        <v>3.0924</v>
+      </c>
+      <c r="C50">
+        <v>50</v>
+      </c>
+      <c r="D50" t="s">
+        <v>1701</v>
+      </c>
+      <c r="E50" t="s">
+        <v>1702</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>101.66868055555599</v>
+      </c>
+      <c r="B51">
+        <v>3.17157222222222</v>
+      </c>
+      <c r="C51">
+        <v>51</v>
+      </c>
+      <c r="D51" t="s">
+        <v>1703</v>
+      </c>
+      <c r="E51" t="s">
+        <v>1704</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>100.37479166666699</v>
+      </c>
+      <c r="B52">
+        <v>5.3894777777777803</v>
+      </c>
+      <c r="C52">
+        <v>52</v>
+      </c>
+      <c r="D52" t="s">
+        <v>1705</v>
+      </c>
+      <c r="E52" t="s">
+        <v>1706</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>101.522327777778</v>
+      </c>
+      <c r="B53">
+        <v>3.1162416666666699</v>
+      </c>
+      <c r="C53">
+        <v>53</v>
+      </c>
+      <c r="D53" t="s">
+        <v>1608</v>
+      </c>
+      <c r="E53" t="s">
+        <v>1707</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>101.721318173211</v>
+      </c>
+      <c r="B54">
+        <v>3.1579250000000001</v>
+      </c>
+      <c r="C54">
+        <v>54</v>
+      </c>
+      <c r="D54" t="s">
+        <v>1611</v>
+      </c>
+      <c r="E54" t="s">
+        <v>1612</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>101.642388888889</v>
+      </c>
+      <c r="B55">
+        <v>3.2101944444444399</v>
+      </c>
+      <c r="C55">
+        <v>55</v>
+      </c>
+      <c r="D55" t="s">
+        <v>1613</v>
+      </c>
+      <c r="E55" t="s">
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>101.46099080969699</v>
+      </c>
+      <c r="B56">
+        <v>2.9708643830146801</v>
+      </c>
+      <c r="C56">
+        <v>56</v>
+      </c>
+      <c r="D56" t="s">
+        <v>1615</v>
+      </c>
+      <c r="E56" t="s">
+        <v>1616</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>100.31079888201999</v>
+      </c>
+      <c r="B57">
+        <v>5.3321057681908304</v>
+      </c>
+      <c r="C57">
+        <v>57</v>
+      </c>
+      <c r="D57" t="s">
+        <v>1617</v>
+      </c>
+      <c r="E57" t="s">
+        <v>1618</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>101.754221851107</v>
+      </c>
+      <c r="B58">
+        <v>2.9988599116086299</v>
+      </c>
+      <c r="C58">
+        <v>58</v>
+      </c>
+      <c r="D58" t="s">
+        <v>1619</v>
+      </c>
+      <c r="E58" t="s">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>101.736906173387</v>
+      </c>
+      <c r="B59">
+        <v>3.19259166666667</v>
+      </c>
+      <c r="C59">
+        <v>59</v>
+      </c>
+      <c r="D59" t="s">
+        <v>1621</v>
+      </c>
+      <c r="E59" t="s">
+        <v>1708</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>101.755873700831</v>
+      </c>
+      <c r="B60">
+        <v>2.9960222004371899</v>
+      </c>
+      <c r="C60">
+        <v>60</v>
+      </c>
+      <c r="D60" t="s">
+        <v>1623</v>
+      </c>
+      <c r="E60" t="s">
+        <v>1709</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>101.755816414771</v>
+      </c>
+      <c r="B61">
+        <v>3.00176388888889</v>
+      </c>
+      <c r="C61">
+        <v>61</v>
+      </c>
+      <c r="D61" t="s">
+        <v>1625</v>
+      </c>
+      <c r="E61" t="s">
+        <v>1626</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>101.79734166666699</v>
+      </c>
+      <c r="B62">
+        <v>2.9211555555555599</v>
+      </c>
+      <c r="C62">
+        <v>62</v>
+      </c>
+      <c r="D62" t="s">
+        <v>1627</v>
+      </c>
+      <c r="E62" t="s">
+        <v>1710</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>100.371392952373</v>
+      </c>
+      <c r="B63">
+        <v>5.4312633333092997</v>
+      </c>
+      <c r="C63">
+        <v>63</v>
+      </c>
+      <c r="D63" t="s">
+        <v>1629</v>
+      </c>
+      <c r="E63" t="s">
+        <v>1630</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>115.495166666667</v>
+      </c>
+      <c r="B64">
+        <v>4.28508333333333</v>
+      </c>
+      <c r="C64">
+        <v>64</v>
+      </c>
+      <c r="D64" t="s">
+        <v>1631</v>
+      </c>
+      <c r="E64" t="s">
+        <v>1632</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>101.413580006853</v>
+      </c>
+      <c r="B65">
+        <v>3.1027349075927102</v>
+      </c>
+      <c r="C65">
+        <v>65</v>
+      </c>
+      <c r="D65" t="s">
+        <v>1633</v>
+      </c>
+      <c r="E65" t="s">
+        <v>1634</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>102.135175599516</v>
+      </c>
+      <c r="B66">
+        <v>2.2753854774955098</v>
+      </c>
+      <c r="C66">
+        <v>66</v>
+      </c>
+      <c r="D66" t="s">
+        <v>1635</v>
+      </c>
+      <c r="E66" t="s">
+        <v>1636</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>101.448710529566</v>
+      </c>
+      <c r="B67">
+        <v>3.1094766836751</v>
+      </c>
+      <c r="C67">
+        <v>67</v>
+      </c>
+      <c r="D67" t="s">
+        <v>1637</v>
+      </c>
+      <c r="E67" t="s">
+        <v>1711</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>101.500553540545</v>
+      </c>
+      <c r="B68">
+        <v>3.1711628199886901</v>
+      </c>
+      <c r="C68">
+        <v>68</v>
+      </c>
+      <c r="D68" t="s">
+        <v>1639</v>
+      </c>
+      <c r="E68" t="s">
+        <v>1640</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>103.31847500000001</v>
+      </c>
+      <c r="B69">
+        <v>2.03000277777778</v>
+      </c>
+      <c r="C69">
+        <v>69</v>
+      </c>
+      <c r="D69" t="s">
+        <v>1641</v>
+      </c>
+      <c r="E69" t="s">
+        <v>1642</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>101.87005609469701</v>
+      </c>
+      <c r="B70">
+        <v>2.9431088301614801</v>
+      </c>
+      <c r="C70">
+        <v>70</v>
+      </c>
+      <c r="D70" t="s">
+        <v>1643</v>
+      </c>
+      <c r="E70" t="s">
+        <v>1712</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>101.718620000006</v>
+      </c>
+      <c r="B71">
+        <v>3.1400799999937501</v>
+      </c>
+      <c r="C71">
+        <v>71</v>
+      </c>
+      <c r="D71" t="s">
+        <v>1645</v>
+      </c>
+      <c r="E71" t="s">
+        <v>1646</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>101.88354722222201</v>
+      </c>
+      <c r="B72">
+        <v>2.9099916666666701</v>
+      </c>
+      <c r="C72">
+        <v>72</v>
+      </c>
+      <c r="D72" t="s">
+        <v>1647</v>
+      </c>
+      <c r="E72" t="s">
+        <v>1648</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>101.71223580399401</v>
+      </c>
+      <c r="B73">
+        <v>3.1339689441857601</v>
+      </c>
+      <c r="C73">
+        <v>73</v>
+      </c>
+      <c r="D73" t="s">
+        <v>1649</v>
+      </c>
+      <c r="E73" t="s">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>100.256471874721</v>
+      </c>
+      <c r="B74">
+        <v>5.3001549762561204</v>
+      </c>
+      <c r="C74">
+        <v>74</v>
+      </c>
+      <c r="D74" t="s">
+        <v>1651</v>
+      </c>
+      <c r="E74" t="s">
+        <v>1652</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>101.19647543137501</v>
+      </c>
+      <c r="B75">
+        <v>4.2053316880020297</v>
+      </c>
+      <c r="C75">
+        <v>75</v>
+      </c>
+      <c r="D75" t="s">
+        <v>1653</v>
+      </c>
+      <c r="E75" t="s">
+        <v>1654</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>101.52394700000001</v>
+      </c>
+      <c r="B76">
+        <v>2.914018</v>
+      </c>
+      <c r="C76">
+        <v>76</v>
+      </c>
+      <c r="D76" t="s">
+        <v>1655</v>
+      </c>
+      <c r="E76" t="s">
+        <v>1656</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>101.035922222222</v>
+      </c>
+      <c r="B77">
+        <v>5.5253361111111099</v>
+      </c>
+      <c r="C77">
+        <v>77</v>
+      </c>
+      <c r="D77" t="s">
+        <v>1657</v>
+      </c>
+      <c r="E77" t="s">
+        <v>1658</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>101.362702777778</v>
+      </c>
+      <c r="B78">
+        <v>2.9742999999999999</v>
+      </c>
+      <c r="C78">
+        <v>78</v>
+      </c>
+      <c r="D78" t="s">
+        <v>1659</v>
+      </c>
+      <c r="E78" t="s">
+        <v>1660</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>100.431811111111</v>
+      </c>
+      <c r="B79">
+        <v>5.2386111111111102</v>
+      </c>
+      <c r="C79">
+        <v>79</v>
+      </c>
+      <c r="D79" t="s">
+        <v>1661</v>
+      </c>
+      <c r="E79" t="s">
+        <v>1662</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>101.654180555556</v>
+      </c>
+      <c r="B80">
+        <v>3.2244555555555601</v>
+      </c>
+      <c r="C80">
+        <v>80</v>
+      </c>
+      <c r="D80" t="s">
+        <v>1663</v>
+      </c>
+      <c r="E80" t="s">
+        <v>1664</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>101.542266666667</v>
+      </c>
+      <c r="B81">
+        <v>3.0509972222222199</v>
+      </c>
+      <c r="C81">
+        <v>81</v>
+      </c>
+      <c r="D81" t="s">
+        <v>1665</v>
+      </c>
+      <c r="E81" t="s">
+        <v>1666</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>101.849952777778</v>
+      </c>
+      <c r="B82">
+        <v>2.8932222222222199</v>
+      </c>
+      <c r="C82">
+        <v>82</v>
+      </c>
+      <c r="D82" t="s">
+        <v>1667</v>
+      </c>
+      <c r="E82" t="s">
+        <v>1668</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>103.68018333333301</v>
+      </c>
+      <c r="B83">
+        <v>1.59805</v>
+      </c>
+      <c r="C83">
+        <v>83</v>
+      </c>
+      <c r="D83" t="s">
+        <v>1669</v>
+      </c>
+      <c r="E83" t="s">
+        <v>1713</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>100.613616666667</v>
+      </c>
+      <c r="B84">
+        <v>5.6596055555555598</v>
+      </c>
+      <c r="C84">
+        <v>84</v>
+      </c>
+      <c r="D84" t="s">
+        <v>1671</v>
+      </c>
+      <c r="E84" t="s">
+        <v>1714</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>101.62524444444399</v>
+      </c>
+      <c r="B85">
+        <v>2.76979166666667</v>
+      </c>
+      <c r="C85">
+        <v>85</v>
+      </c>
+      <c r="D85" t="s">
+        <v>1673</v>
+      </c>
+      <c r="E85" t="s">
+        <v>1674</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>101.154016666667</v>
+      </c>
+      <c r="B86">
+        <v>4.5289805555555596</v>
+      </c>
+      <c r="C86">
+        <v>86</v>
+      </c>
+      <c r="D86" t="s">
+        <v>1675</v>
+      </c>
+      <c r="E86" t="s">
+        <v>1676</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>103.590858333333</v>
+      </c>
+      <c r="B87">
+        <v>1.43166666666667</v>
+      </c>
+      <c r="C87">
+        <v>87</v>
+      </c>
+      <c r="D87" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E87" t="s">
+        <v>1678</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>104.111111111111</v>
+      </c>
+      <c r="B88">
+        <v>1.36470277777778</v>
+      </c>
+      <c r="C88">
+        <v>88</v>
+      </c>
+      <c r="D88" t="s">
+        <v>1679</v>
+      </c>
+      <c r="E88" t="s">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>69.569105555555595</v>
+      </c>
+      <c r="B89">
+        <v>24.0290416666667</v>
+      </c>
+      <c r="C89">
+        <v>89</v>
+      </c>
+      <c r="D89" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E89" t="s">
+        <v>1682</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>101.715363888889</v>
+      </c>
+      <c r="B90">
+        <v>3.2033083333333301</v>
+      </c>
+      <c r="C90">
+        <v>90</v>
+      </c>
+      <c r="D90" t="s">
+        <v>1683</v>
+      </c>
+      <c r="E90" t="s">
+        <v>1684</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>100.396916666667</v>
+      </c>
+      <c r="B91">
+        <v>5.3953527777777799</v>
+      </c>
+      <c r="C91">
+        <v>91</v>
+      </c>
+      <c r="D91" t="s">
+        <v>1685</v>
+      </c>
+      <c r="E91" t="s">
+        <v>1686</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>101.154016666667</v>
+      </c>
+      <c r="B92">
+        <v>4.5289805555555596</v>
+      </c>
+      <c r="C92">
+        <v>92</v>
+      </c>
+      <c r="D92" t="s">
+        <v>1687</v>
+      </c>
+      <c r="E92" t="s">
+        <v>1715</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>101.461252777778</v>
+      </c>
+      <c r="B93">
+        <v>2.9946305555555601</v>
+      </c>
+      <c r="C93">
+        <v>93</v>
+      </c>
+      <c r="D93" t="s">
+        <v>1689</v>
+      </c>
+      <c r="E93" t="s">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>101.708652777778</v>
+      </c>
+      <c r="B94">
+        <v>3.11690277777778</v>
+      </c>
+      <c r="C94">
+        <v>94</v>
+      </c>
+      <c r="D94" t="s">
+        <v>1716</v>
+      </c>
+      <c r="E94" t="s">
+        <v>1717</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>100.37479166666699</v>
+      </c>
+      <c r="B95">
+        <v>5.3894777777777803</v>
+      </c>
+      <c r="C95">
+        <v>95</v>
+      </c>
+      <c r="D95" t="s">
+        <v>1705</v>
+      </c>
+      <c r="E95" t="s">
+        <v>1718</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>101.66868055555599</v>
+      </c>
+      <c r="B96">
+        <v>3.17157222222222</v>
+      </c>
+      <c r="C96">
+        <v>96</v>
+      </c>
+      <c r="D96" t="s">
+        <v>1703</v>
+      </c>
+      <c r="E96" t="s">
+        <v>1719</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>101.882469444444</v>
+      </c>
+      <c r="B97">
+        <v>3.0769195419896098</v>
+      </c>
+      <c r="C97">
+        <v>1</v>
+      </c>
+      <c r="D97" t="s">
+        <v>1604</v>
+      </c>
+      <c r="E97" t="s">
+        <v>1605</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>108.3035</v>
+      </c>
+      <c r="B98">
+        <v>4.1458250975451598</v>
+      </c>
+      <c r="C98">
+        <v>2</v>
+      </c>
+      <c r="D98" t="s">
+        <v>1606</v>
+      </c>
+      <c r="E98" t="s">
+        <v>1607</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>101.522327777778</v>
+      </c>
+      <c r="B99">
+        <v>3.1162417642118299</v>
+      </c>
+      <c r="C99">
+        <v>3</v>
+      </c>
+      <c r="D99" t="s">
+        <v>1608</v>
+      </c>
+      <c r="E99" t="s">
+        <v>1609</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>101.88246807070701</v>
+      </c>
+      <c r="B100">
+        <v>3.07691819776633</v>
+      </c>
+      <c r="C100">
+        <v>4</v>
+      </c>
+      <c r="D100" t="s">
+        <v>1604</v>
+      </c>
+      <c r="E100" t="s">
+        <v>1610</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>101.721318173211</v>
+      </c>
+      <c r="B101">
+        <v>3.15792509754516</v>
+      </c>
+      <c r="C101">
+        <v>5</v>
+      </c>
+      <c r="D101" t="s">
+        <v>1611</v>
+      </c>
+      <c r="E101" t="s">
+        <v>1612</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>101.642388888889</v>
+      </c>
+      <c r="B102">
+        <v>3.2101945419896101</v>
+      </c>
+      <c r="C102">
+        <v>6</v>
+      </c>
+      <c r="D102" t="s">
+        <v>1613</v>
+      </c>
+      <c r="E102" t="s">
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>101.46099080969699</v>
+      </c>
+      <c r="B103">
+        <v>2.9708644805598401</v>
+      </c>
+      <c r="C103">
+        <v>7</v>
+      </c>
+      <c r="D103" t="s">
+        <v>1615</v>
+      </c>
+      <c r="E103" t="s">
+        <v>1616</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>100.31079888201999</v>
+      </c>
+      <c r="B104">
+        <v>5.3321058657359899</v>
+      </c>
+      <c r="C104">
+        <v>8</v>
+      </c>
+      <c r="D104" t="s">
+        <v>1617</v>
+      </c>
+      <c r="E104" t="s">
+        <v>1618</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>101.754221851107</v>
+      </c>
+      <c r="B105">
+        <v>2.9988600091537898</v>
+      </c>
+      <c r="C105">
+        <v>9</v>
+      </c>
+      <c r="D105" t="s">
+        <v>1619</v>
+      </c>
+      <c r="E105" t="s">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>101.736906173387</v>
+      </c>
+      <c r="B106">
+        <v>3.19259176421183</v>
+      </c>
+      <c r="C106">
+        <v>10</v>
+      </c>
+      <c r="D106" t="s">
+        <v>1621</v>
+      </c>
+      <c r="E106" t="s">
+        <v>1622</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>101.755873700831</v>
+      </c>
+      <c r="B107">
+        <v>2.9960222979823499</v>
+      </c>
+      <c r="C107">
+        <v>11</v>
+      </c>
+      <c r="D107" t="s">
+        <v>1623</v>
+      </c>
+      <c r="E107" t="s">
+        <v>1624</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <v>101.755816414771</v>
+      </c>
+      <c r="B108">
+        <v>3.00176398643405</v>
+      </c>
+      <c r="C108">
+        <v>12</v>
+      </c>
+      <c r="D108" t="s">
+        <v>1625</v>
+      </c>
+      <c r="E108" t="s">
+        <v>1626</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <v>101.79734166666699</v>
+      </c>
+      <c r="B109">
+        <v>2.9211556531007199</v>
+      </c>
+      <c r="C109">
+        <v>13</v>
+      </c>
+      <c r="D109" t="s">
+        <v>1627</v>
+      </c>
+      <c r="E109" t="s">
+        <v>1628</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <v>100.371392952373</v>
+      </c>
+      <c r="B110">
+        <v>5.4312634308544601</v>
+      </c>
+      <c r="C110">
+        <v>14</v>
+      </c>
+      <c r="D110" t="s">
+        <v>1629</v>
+      </c>
+      <c r="E110" t="s">
+        <v>1630</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <v>115.495166666667</v>
+      </c>
+      <c r="B111">
+        <v>4.2850834308784904</v>
+      </c>
+      <c r="C111">
+        <v>15</v>
+      </c>
+      <c r="D111" t="s">
+        <v>1631</v>
+      </c>
+      <c r="E111" t="s">
+        <v>1632</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <v>101.413580006853</v>
+      </c>
+      <c r="B112">
+        <v>3.1027350051378702</v>
+      </c>
+      <c r="C112">
+        <v>16</v>
+      </c>
+      <c r="D112" t="s">
+        <v>1633</v>
+      </c>
+      <c r="E112" t="s">
+        <v>1634</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <v>102.135175599516</v>
+      </c>
+      <c r="B113">
+        <v>2.2753855750406702</v>
+      </c>
+      <c r="C113">
+        <v>17</v>
+      </c>
+      <c r="D113" t="s">
+        <v>1635</v>
+      </c>
+      <c r="E113" t="s">
+        <v>1636</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>101.448710529566</v>
+      </c>
+      <c r="B114">
+        <v>3.1094767812202599</v>
+      </c>
+      <c r="C114">
+        <v>18</v>
+      </c>
+      <c r="D114" t="s">
+        <v>1637</v>
+      </c>
+      <c r="E114" t="s">
+        <v>1638</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>101.500553540545</v>
+      </c>
+      <c r="B115">
+        <v>3.17116291753385</v>
+      </c>
+      <c r="C115">
+        <v>19</v>
+      </c>
+      <c r="D115" t="s">
+        <v>1639</v>
+      </c>
+      <c r="E115" t="s">
+        <v>1640</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <v>103.31847500000001</v>
+      </c>
+      <c r="B116">
+        <v>2.03000287532294</v>
+      </c>
+      <c r="C116">
+        <v>20</v>
+      </c>
+      <c r="D116" t="s">
+        <v>1641</v>
+      </c>
+      <c r="E116" t="s">
+        <v>1642</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <v>101.87005609469701</v>
+      </c>
+      <c r="B117">
+        <v>2.9431089277066498</v>
+      </c>
+      <c r="C117">
+        <v>21</v>
+      </c>
+      <c r="D117" t="s">
+        <v>1643</v>
+      </c>
+      <c r="E117" t="s">
+        <v>1644</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>101.718620000006</v>
+      </c>
+      <c r="B118">
+        <v>3.1400800975389198</v>
+      </c>
+      <c r="C118">
+        <v>22</v>
+      </c>
+      <c r="D118" t="s">
+        <v>1645</v>
+      </c>
+      <c r="E118" t="s">
+        <v>1646</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>101.88354722222201</v>
+      </c>
+      <c r="B119">
+        <v>2.90999176421183</v>
+      </c>
+      <c r="C119">
+        <v>23</v>
+      </c>
+      <c r="D119" t="s">
+        <v>1647</v>
+      </c>
+      <c r="E119" t="s">
+        <v>1648</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <v>101.71223580399401</v>
+      </c>
+      <c r="B120">
+        <v>3.1339690417309201</v>
+      </c>
+      <c r="C120">
+        <v>24</v>
+      </c>
+      <c r="D120" t="s">
+        <v>1649</v>
+      </c>
+      <c r="E120" t="s">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <v>100.256471874721</v>
+      </c>
+      <c r="B121">
+        <v>5.3001550738012897</v>
+      </c>
+      <c r="C121">
+        <v>25</v>
+      </c>
+      <c r="D121" t="s">
+        <v>1651</v>
+      </c>
+      <c r="E121" t="s">
+        <v>1652</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A122">
+        <v>101.19647543137501</v>
+      </c>
+      <c r="B122">
+        <v>4.2053317855471901</v>
+      </c>
+      <c r="C122">
+        <v>26</v>
+      </c>
+      <c r="D122" t="s">
+        <v>1653</v>
+      </c>
+      <c r="E122" t="s">
+        <v>1654</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A123">
+        <v>101.52394700000001</v>
+      </c>
+      <c r="B123">
+        <v>2.9140180975451599</v>
+      </c>
+      <c r="C123">
+        <v>27</v>
+      </c>
+      <c r="D123" t="s">
+        <v>1655</v>
+      </c>
+      <c r="E123" t="s">
+        <v>1656</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A124">
+        <v>101.035922222222</v>
+      </c>
+      <c r="B124">
+        <v>5.5253362086562703</v>
+      </c>
+      <c r="C124">
+        <v>28</v>
+      </c>
+      <c r="D124" t="s">
+        <v>1657</v>
+      </c>
+      <c r="E124" t="s">
+        <v>1658</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A125">
+        <v>101.362702777778</v>
+      </c>
+      <c r="B125">
+        <v>2.9743000975451599</v>
+      </c>
+      <c r="C125">
+        <v>29</v>
+      </c>
+      <c r="D125" t="s">
+        <v>1659</v>
+      </c>
+      <c r="E125" t="s">
+        <v>1660</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <v>100.431811111111</v>
+      </c>
+      <c r="B126">
+        <v>5.2386112086562697</v>
+      </c>
+      <c r="C126">
+        <v>30</v>
+      </c>
+      <c r="D126" t="s">
+        <v>1661</v>
+      </c>
+      <c r="E126" t="s">
+        <v>1662</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A127">
+        <v>101.654180555556</v>
+      </c>
+      <c r="B127">
+        <v>3.22445565310072</v>
+      </c>
+      <c r="C127">
+        <v>31</v>
+      </c>
+      <c r="D127" t="s">
+        <v>1663</v>
+      </c>
+      <c r="E127" t="s">
+        <v>1664</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <v>101.542266666667</v>
+      </c>
+      <c r="B128">
+        <v>3.0509973197673799</v>
+      </c>
+      <c r="C128">
+        <v>32</v>
+      </c>
+      <c r="D128" t="s">
+        <v>1665</v>
+      </c>
+      <c r="E128" t="s">
+        <v>1666</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <v>101.849952777778</v>
+      </c>
+      <c r="B129">
+        <v>2.8932223197673799</v>
+      </c>
+      <c r="C129">
+        <v>33</v>
+      </c>
+      <c r="D129" t="s">
+        <v>1667</v>
+      </c>
+      <c r="E129" t="s">
+        <v>1668</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A130">
+        <v>103.68018333333301</v>
+      </c>
+      <c r="B130">
+        <v>1.5980500975451599</v>
+      </c>
+      <c r="C130">
+        <v>34</v>
+      </c>
+      <c r="D130" t="s">
+        <v>1669</v>
+      </c>
+      <c r="E130" t="s">
+        <v>1670</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A131">
+        <v>100.613616666667</v>
+      </c>
+      <c r="B131">
+        <v>5.6596056531007202</v>
+      </c>
+      <c r="C131">
+        <v>35</v>
+      </c>
+      <c r="D131" t="s">
+        <v>1671</v>
+      </c>
+      <c r="E131" t="s">
+        <v>1672</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A132">
+        <v>101.62524444444399</v>
+      </c>
+      <c r="B132">
+        <v>2.7697917642118299</v>
+      </c>
+      <c r="C132">
+        <v>36</v>
+      </c>
+      <c r="D132" t="s">
+        <v>1673</v>
+      </c>
+      <c r="E132" t="s">
+        <v>1674</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A133">
+        <v>101.154016666667</v>
+      </c>
+      <c r="B133">
+        <v>4.52898065310072</v>
+      </c>
+      <c r="C133">
+        <v>37</v>
+      </c>
+      <c r="D133" t="s">
+        <v>1675</v>
+      </c>
+      <c r="E133" t="s">
+        <v>1676</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A134">
+        <v>103.590858333333</v>
+      </c>
+      <c r="B134">
+        <v>1.4316667642118299</v>
+      </c>
+      <c r="C134">
+        <v>38</v>
+      </c>
+      <c r="D134" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E134" t="s">
+        <v>1678</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A135">
+        <v>104.111111111111</v>
+      </c>
+      <c r="B135">
+        <v>1.36470287532294</v>
+      </c>
+      <c r="C135">
+        <v>39</v>
+      </c>
+      <c r="D135" t="s">
+        <v>1679</v>
+      </c>
+      <c r="E135" t="s">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <v>69.569105555555595</v>
+      </c>
+      <c r="B136">
+        <v>24.029041764211801</v>
+      </c>
+      <c r="C136">
+        <v>40</v>
+      </c>
+      <c r="D136" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E136" t="s">
+        <v>1682</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A137">
+        <v>101.715363888889</v>
+      </c>
+      <c r="B137">
+        <v>3.2033084308784998</v>
+      </c>
+      <c r="C137">
+        <v>41</v>
+      </c>
+      <c r="D137" t="s">
+        <v>1683</v>
+      </c>
+      <c r="E137" t="s">
+        <v>1684</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A138">
+        <v>100.396916666667</v>
+      </c>
+      <c r="B138">
+        <v>5.3953528753229403</v>
+      </c>
+      <c r="C138">
+        <v>42</v>
+      </c>
+      <c r="D138" t="s">
+        <v>1685</v>
+      </c>
+      <c r="E138" t="s">
+        <v>1686</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A139">
+        <v>101.154016666667</v>
+      </c>
+      <c r="B139">
+        <v>4.52898065310072</v>
+      </c>
+      <c r="C139">
+        <v>43</v>
+      </c>
+      <c r="D139" t="s">
+        <v>1687</v>
+      </c>
+      <c r="E139" t="s">
+        <v>1688</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A140">
+        <v>101.461252777778</v>
+      </c>
+      <c r="B140">
+        <v>2.9946306531007201</v>
+      </c>
+      <c r="C140">
+        <v>44</v>
+      </c>
+      <c r="D140" t="s">
+        <v>1689</v>
+      </c>
+      <c r="E140" t="s">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A141">
+        <v>101.68220833333299</v>
+      </c>
+      <c r="B141">
+        <v>3.2318834308784998</v>
+      </c>
+      <c r="C141">
+        <v>45</v>
+      </c>
+      <c r="D141" t="s">
+        <v>1691</v>
+      </c>
+      <c r="E141" t="s">
+        <v>1692</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A142">
+        <v>101.436333333333</v>
+      </c>
+      <c r="B142">
+        <v>3.2354973197673802</v>
+      </c>
+      <c r="C142">
+        <v>46</v>
+      </c>
+      <c r="D142" t="s">
+        <v>1693</v>
+      </c>
+      <c r="E142" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A143">
+        <v>101.154016666667</v>
+      </c>
+      <c r="B143">
+        <v>4.52898065310072</v>
+      </c>
+      <c r="C143">
+        <v>47</v>
+      </c>
+      <c r="D143" t="s">
+        <v>1695</v>
+      </c>
+      <c r="E143" t="s">
+        <v>1696</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A144">
+        <v>101.59655833333299</v>
+      </c>
+      <c r="B144">
+        <v>3.1501028753229399</v>
+      </c>
+      <c r="C144">
+        <v>48</v>
+      </c>
+      <c r="D144" t="s">
+        <v>1697</v>
+      </c>
+      <c r="E144" t="s">
+        <v>1698</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A145">
+        <v>101.68445</v>
+      </c>
+      <c r="B145">
+        <v>3.0896056531007199</v>
+      </c>
+      <c r="C145">
+        <v>49</v>
+      </c>
+      <c r="D145" t="s">
+        <v>1699</v>
+      </c>
+      <c r="E145" t="s">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A146">
+        <v>101.45906388888901</v>
+      </c>
+      <c r="B146">
+        <v>3.09240009754516</v>
+      </c>
+      <c r="C146">
+        <v>50</v>
+      </c>
+      <c r="D146" t="s">
+        <v>1701</v>
+      </c>
+      <c r="E146" t="s">
+        <v>1702</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A147">
+        <v>101.66868055555599</v>
+      </c>
+      <c r="B147">
+        <v>3.17157231976738</v>
+      </c>
+      <c r="C147">
+        <v>51</v>
+      </c>
+      <c r="D147" t="s">
+        <v>1703</v>
+      </c>
+      <c r="E147" t="s">
+        <v>1704</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A148">
+        <v>100.37479166666699</v>
+      </c>
+      <c r="B148">
+        <v>5.3894778753229398</v>
+      </c>
+      <c r="C148">
+        <v>52</v>
+      </c>
+      <c r="D148" t="s">
+        <v>1705</v>
+      </c>
+      <c r="E148" t="s">
+        <v>1706</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A149">
+        <v>101.522327777778</v>
+      </c>
+      <c r="B149">
+        <v>3.1162417642118299</v>
+      </c>
+      <c r="C149">
+        <v>53</v>
+      </c>
+      <c r="D149" t="s">
+        <v>1608</v>
+      </c>
+      <c r="E149" t="s">
+        <v>1707</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A150">
+        <v>101.721318173211</v>
+      </c>
+      <c r="B150">
+        <v>3.15792509754516</v>
+      </c>
+      <c r="C150">
+        <v>54</v>
+      </c>
+      <c r="D150" t="s">
+        <v>1611</v>
+      </c>
+      <c r="E150" t="s">
+        <v>1612</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A151">
+        <v>101.642388888889</v>
+      </c>
+      <c r="B151">
+        <v>3.2101945419896101</v>
+      </c>
+      <c r="C151">
+        <v>55</v>
+      </c>
+      <c r="D151" t="s">
+        <v>1613</v>
+      </c>
+      <c r="E151" t="s">
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A152">
+        <v>101.46099080969699</v>
+      </c>
+      <c r="B152">
+        <v>2.9708644805598401</v>
+      </c>
+      <c r="C152">
+        <v>56</v>
+      </c>
+      <c r="D152" t="s">
+        <v>1615</v>
+      </c>
+      <c r="E152" t="s">
+        <v>1616</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A153">
+        <v>100.31079888201999</v>
+      </c>
+      <c r="B153">
+        <v>5.3321058657359899</v>
+      </c>
+      <c r="C153">
+        <v>57</v>
+      </c>
+      <c r="D153" t="s">
+        <v>1617</v>
+      </c>
+      <c r="E153" t="s">
+        <v>1618</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A154">
+        <v>101.754221851107</v>
+      </c>
+      <c r="B154">
+        <v>2.9988600091537898</v>
+      </c>
+      <c r="C154">
+        <v>58</v>
+      </c>
+      <c r="D154" t="s">
+        <v>1619</v>
+      </c>
+      <c r="E154" t="s">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A155">
+        <v>101.736906173387</v>
+      </c>
+      <c r="B155">
+        <v>3.19259176421183</v>
+      </c>
+      <c r="C155">
+        <v>59</v>
+      </c>
+      <c r="D155" t="s">
+        <v>1621</v>
+      </c>
+      <c r="E155" t="s">
+        <v>1708</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A156">
+        <v>101.755873700831</v>
+      </c>
+      <c r="B156">
+        <v>2.9960222979823499</v>
+      </c>
+      <c r="C156">
+        <v>60</v>
+      </c>
+      <c r="D156" t="s">
+        <v>1623</v>
+      </c>
+      <c r="E156" t="s">
+        <v>1709</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A157">
+        <v>101.755816414771</v>
+      </c>
+      <c r="B157">
+        <v>3.00176398643405</v>
+      </c>
+      <c r="C157">
+        <v>61</v>
+      </c>
+      <c r="D157" t="s">
+        <v>1625</v>
+      </c>
+      <c r="E157" t="s">
+        <v>1626</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A158">
+        <v>101.79734166666699</v>
+      </c>
+      <c r="B158">
+        <v>2.9211556531007199</v>
+      </c>
+      <c r="C158">
+        <v>62</v>
+      </c>
+      <c r="D158" t="s">
+        <v>1627</v>
+      </c>
+      <c r="E158" t="s">
+        <v>1710</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A159">
+        <v>100.371392952373</v>
+      </c>
+      <c r="B159">
+        <v>5.4312634308544601</v>
+      </c>
+      <c r="C159">
+        <v>63</v>
+      </c>
+      <c r="D159" t="s">
+        <v>1629</v>
+      </c>
+      <c r="E159" t="s">
+        <v>1630</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A160">
+        <v>115.495166666667</v>
+      </c>
+      <c r="B160">
+        <v>4.2850834308784904</v>
+      </c>
+      <c r="C160">
+        <v>64</v>
+      </c>
+      <c r="D160" t="s">
+        <v>1631</v>
+      </c>
+      <c r="E160" t="s">
+        <v>1632</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A161">
+        <v>101.413580006853</v>
+      </c>
+      <c r="B161">
+        <v>3.1027350051378702</v>
+      </c>
+      <c r="C161">
+        <v>65</v>
+      </c>
+      <c r="D161" t="s">
+        <v>1633</v>
+      </c>
+      <c r="E161" t="s">
+        <v>1634</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A162">
+        <v>102.135175599516</v>
+      </c>
+      <c r="B162">
+        <v>2.2753855750406702</v>
+      </c>
+      <c r="C162">
+        <v>66</v>
+      </c>
+      <c r="D162" t="s">
+        <v>1635</v>
+      </c>
+      <c r="E162" t="s">
+        <v>1636</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A163">
+        <v>101.448710529566</v>
+      </c>
+      <c r="B163">
+        <v>3.1094767812202599</v>
+      </c>
+      <c r="C163">
+        <v>67</v>
+      </c>
+      <c r="D163" t="s">
+        <v>1637</v>
+      </c>
+      <c r="E163" t="s">
+        <v>1711</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A164">
+        <v>101.500553540545</v>
+      </c>
+      <c r="B164">
+        <v>3.17116291753385</v>
+      </c>
+      <c r="C164">
+        <v>68</v>
+      </c>
+      <c r="D164" t="s">
+        <v>1639</v>
+      </c>
+      <c r="E164" t="s">
+        <v>1640</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A165">
+        <v>103.31847500000001</v>
+      </c>
+      <c r="B165">
+        <v>2.03000287532294</v>
+      </c>
+      <c r="C165">
+        <v>69</v>
+      </c>
+      <c r="D165" t="s">
+        <v>1641</v>
+      </c>
+      <c r="E165" t="s">
+        <v>1642</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A166">
+        <v>101.87005609469701</v>
+      </c>
+      <c r="B166">
+        <v>2.9431089277066498</v>
+      </c>
+      <c r="C166">
+        <v>70</v>
+      </c>
+      <c r="D166" t="s">
+        <v>1643</v>
+      </c>
+      <c r="E166" t="s">
+        <v>1712</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A167">
+        <v>101.718620000006</v>
+      </c>
+      <c r="B167">
+        <v>3.1400800975389198</v>
+      </c>
+      <c r="C167">
+        <v>71</v>
+      </c>
+      <c r="D167" t="s">
+        <v>1645</v>
+      </c>
+      <c r="E167" t="s">
+        <v>1646</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A168">
+        <v>101.88354722222201</v>
+      </c>
+      <c r="B168">
+        <v>2.90999176421183</v>
+      </c>
+      <c r="C168">
+        <v>72</v>
+      </c>
+      <c r="D168" t="s">
+        <v>1647</v>
+      </c>
+      <c r="E168" t="s">
+        <v>1648</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A169">
+        <v>101.71223580399401</v>
+      </c>
+      <c r="B169">
+        <v>3.1339690417309201</v>
+      </c>
+      <c r="C169">
+        <v>73</v>
+      </c>
+      <c r="D169" t="s">
+        <v>1649</v>
+      </c>
+      <c r="E169" t="s">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A170">
+        <v>100.256471874721</v>
+      </c>
+      <c r="B170">
+        <v>5.3001550738012897</v>
+      </c>
+      <c r="C170">
+        <v>74</v>
+      </c>
+      <c r="D170" t="s">
+        <v>1651</v>
+      </c>
+      <c r="E170" t="s">
+        <v>1652</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A171">
+        <v>101.19647543137501</v>
+      </c>
+      <c r="B171">
+        <v>4.2053317855471901</v>
+      </c>
+      <c r="C171">
+        <v>75</v>
+      </c>
+      <c r="D171" t="s">
+        <v>1653</v>
+      </c>
+      <c r="E171" t="s">
+        <v>1654</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A172">
+        <v>101.52394700000001</v>
+      </c>
+      <c r="B172">
+        <v>2.9140180975451599</v>
+      </c>
+      <c r="C172">
+        <v>76</v>
+      </c>
+      <c r="D172" t="s">
+        <v>1655</v>
+      </c>
+      <c r="E172" t="s">
+        <v>1656</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A173">
+        <v>101.035922222222</v>
+      </c>
+      <c r="B173">
+        <v>5.5253362086562703</v>
+      </c>
+      <c r="C173">
+        <v>77</v>
+      </c>
+      <c r="D173" t="s">
+        <v>1657</v>
+      </c>
+      <c r="E173" t="s">
+        <v>1658</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A174">
+        <v>101.362702777778</v>
+      </c>
+      <c r="B174">
+        <v>2.9743000975451599</v>
+      </c>
+      <c r="C174">
+        <v>78</v>
+      </c>
+      <c r="D174" t="s">
+        <v>1659</v>
+      </c>
+      <c r="E174" t="s">
+        <v>1660</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A175">
+        <v>100.431811111111</v>
+      </c>
+      <c r="B175">
+        <v>5.2386112086562697</v>
+      </c>
+      <c r="C175">
+        <v>79</v>
+      </c>
+      <c r="D175" t="s">
+        <v>1661</v>
+      </c>
+      <c r="E175" t="s">
+        <v>1662</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A176">
+        <v>101.654180555556</v>
+      </c>
+      <c r="B176">
+        <v>3.22445565310072</v>
+      </c>
+      <c r="C176">
+        <v>80</v>
+      </c>
+      <c r="D176" t="s">
+        <v>1663</v>
+      </c>
+      <c r="E176" t="s">
+        <v>1664</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A177">
+        <v>101.542266666667</v>
+      </c>
+      <c r="B177">
+        <v>3.0509973197673799</v>
+      </c>
+      <c r="C177">
+        <v>81</v>
+      </c>
+      <c r="D177" t="s">
+        <v>1665</v>
+      </c>
+      <c r="E177" t="s">
+        <v>1666</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A178">
+        <v>101.849952777778</v>
+      </c>
+      <c r="B178">
+        <v>2.8932223197673799</v>
+      </c>
+      <c r="C178">
+        <v>82</v>
+      </c>
+      <c r="D178" t="s">
+        <v>1667</v>
+      </c>
+      <c r="E178" t="s">
+        <v>1668</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A179">
+        <v>103.68018333333301</v>
+      </c>
+      <c r="B179">
+        <v>1.5980500975451599</v>
+      </c>
+      <c r="C179">
+        <v>83</v>
+      </c>
+      <c r="D179" t="s">
+        <v>1669</v>
+      </c>
+      <c r="E179" t="s">
+        <v>1713</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A180">
+        <v>100.613616666667</v>
+      </c>
+      <c r="B180">
+        <v>5.6596056531007202</v>
+      </c>
+      <c r="C180">
+        <v>84</v>
+      </c>
+      <c r="D180" t="s">
+        <v>1671</v>
+      </c>
+      <c r="E180" t="s">
+        <v>1714</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A181">
+        <v>101.62524444444399</v>
+      </c>
+      <c r="B181">
+        <v>2.7697917642118299</v>
+      </c>
+      <c r="C181">
+        <v>85</v>
+      </c>
+      <c r="D181" t="s">
+        <v>1673</v>
+      </c>
+      <c r="E181" t="s">
+        <v>1674</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A182">
+        <v>101.154016666667</v>
+      </c>
+      <c r="B182">
+        <v>4.52898065310072</v>
+      </c>
+      <c r="C182">
+        <v>86</v>
+      </c>
+      <c r="D182" t="s">
+        <v>1675</v>
+      </c>
+      <c r="E182" t="s">
+        <v>1676</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A183">
+        <v>103.590858333333</v>
+      </c>
+      <c r="B183">
+        <v>1.4316667642118299</v>
+      </c>
+      <c r="C183">
+        <v>87</v>
+      </c>
+      <c r="D183" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E183" t="s">
+        <v>1678</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A184">
+        <v>104.111111111111</v>
+      </c>
+      <c r="B184">
+        <v>1.36470287532294</v>
+      </c>
+      <c r="C184">
+        <v>88</v>
+      </c>
+      <c r="D184" t="s">
+        <v>1679</v>
+      </c>
+      <c r="E184" t="s">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A185">
+        <v>69.569105555555595</v>
+      </c>
+      <c r="B185">
+        <v>24.029041764211801</v>
+      </c>
+      <c r="C185">
+        <v>89</v>
+      </c>
+      <c r="D185" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E185" t="s">
+        <v>1682</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A186">
+        <v>101.715363888889</v>
+      </c>
+      <c r="B186">
+        <v>3.2033084308784998</v>
+      </c>
+      <c r="C186">
+        <v>90</v>
+      </c>
+      <c r="D186" t="s">
+        <v>1683</v>
+      </c>
+      <c r="E186" t="s">
+        <v>1684</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A187">
+        <v>100.396916666667</v>
+      </c>
+      <c r="B187">
+        <v>5.3953528753229403</v>
+      </c>
+      <c r="C187">
+        <v>91</v>
+      </c>
+      <c r="D187" t="s">
+        <v>1685</v>
+      </c>
+      <c r="E187" t="s">
+        <v>1686</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A188">
+        <v>101.154016666667</v>
+      </c>
+      <c r="B188">
+        <v>4.52898065310072</v>
+      </c>
+      <c r="C188">
+        <v>92</v>
+      </c>
+      <c r="D188" t="s">
+        <v>1687</v>
+      </c>
+      <c r="E188" t="s">
+        <v>1715</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A189">
+        <v>101.461252777778</v>
+      </c>
+      <c r="B189">
+        <v>2.9946306531007201</v>
+      </c>
+      <c r="C189">
+        <v>93</v>
+      </c>
+      <c r="D189" t="s">
+        <v>1689</v>
+      </c>
+      <c r="E189" t="s">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A190">
+        <v>101.708652777778</v>
+      </c>
+      <c r="B190">
+        <v>3.11690287532294</v>
+      </c>
+      <c r="C190">
+        <v>94</v>
+      </c>
+      <c r="D190" t="s">
+        <v>1716</v>
+      </c>
+      <c r="E190" t="s">
+        <v>1717</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A191">
+        <v>100.37479166666699</v>
+      </c>
+      <c r="B191">
+        <v>5.3894778753229398</v>
+      </c>
+      <c r="C191">
+        <v>95</v>
+      </c>
+      <c r="D191" t="s">
+        <v>1705</v>
+      </c>
+      <c r="E191" t="s">
+        <v>1718</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A192">
+        <v>101.66868055555599</v>
+      </c>
+      <c r="B192">
+        <v>3.17157231976738</v>
+      </c>
+      <c r="C192">
+        <v>96</v>
+      </c>
+      <c r="D192" t="s">
+        <v>1703</v>
+      </c>
+      <c r="E192" t="s">
+        <v>1719</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
commit "Excel Database updating"
</commit_message>
<xml_diff>
--- a/2020_Gallery.xlsx
+++ b/2020_Gallery.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KN\Desktop\SPORTS CLUB 2019-2020\06 Programming\02_Workshop_Material\01_Sphinx\Vir_Pro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D9D3C6-7AE7-425E-BDC6-E174474D80F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1A3FD0A-401C-4491-9422-58654640DEE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2020" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2079" uniqueCount="1702">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2078" uniqueCount="1702">
   <si>
     <t>x</t>
   </si>
@@ -22621,7 +22621,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -22630,6 +22630,12 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -22654,10 +22660,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -24497,7 +24504,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EA44208-C8B0-49AE-B570-043027A362D8}">
   <dimension ref="A1:F99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
@@ -37348,8 +37355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{445AE014-FA9C-4312-821A-C1DFDF2E16BA}">
   <dimension ref="A1:E98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D75" sqref="D75"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39:XFD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -37367,8 +37374,8 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
+      <c r="D1">
+        <v>13</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
@@ -37731,20 +37738,20 @@
         <v>703</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>108.541652777778</v>
-      </c>
-      <c r="B23">
+    <row r="23" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
+        <v>103.541652777778</v>
+      </c>
+      <c r="B23" s="3">
         <v>1.3343055555555501</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="3">
         <v>22</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="3" t="s">
         <v>704</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="3" t="s">
         <v>705</v>
       </c>
     </row>
@@ -38003,20 +38010,20 @@
         <v>729</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39">
+    <row r="39" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="3">
         <v>103.541652252323</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="3">
         <v>1.33430621752081</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="3">
         <v>37</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="3" t="s">
         <v>730</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39" s="3" t="s">
         <v>731</v>
       </c>
     </row>

</xml_diff>